<commit_message>
Docs: solution02 API문서 수정
- 기능 분류, 메소드 명, 받아야할/보내야할 값 수정
</commit_message>
<xml_diff>
--- a/docs/API_문서.xlsx
+++ b/docs/API_문서.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gimhwigyeong/Desktop/hwi/취준/하반기/sakak/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gimhwigyeong/Desktop/hwi/취준/하반기/sakak/tar/programming-test/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C87C3F-E791-A34E-9E76-35B08D59A1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB138E1-573F-5C4D-8D50-94F2E9693CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="1140" windowWidth="28300" windowHeight="16600" xr2:uid="{C04F700B-1A3C-3B45-AB6B-73AAF2520DD4}"/>
+    <workbookView xWindow="2460" yWindow="3140" windowWidth="28300" windowHeight="16600" xr2:uid="{C04F700B-1A3C-3B45-AB6B-73AAF2520DD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>기능 분류</t>
   </si>
@@ -62,9 +62,6 @@
     <t>비고</t>
   </si>
   <si>
-    <t>login</t>
-  </si>
-  <si>
     <t>조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,34 +74,44 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>getFoodInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>{
-    "food_name": "hwi"
-    "research_year": "abc1234",
-    "maker_name": "hwikyung",
-    "food_code": "h 
+    "food_name": "닭갈비"
+    "research_year": "2019",
+    "maker_name": "춘천",
+    "food_code": "D000008" 
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{
-    "id": "hwi"
-    "food_cd": "abc1234",
-    "group_name": "hwikyung",
-    "food_name": "h,
-    "research_year": "h,
-    "maker_name": "h,
-    "ref_name": "h,
-    "serving_size": "h,
-    "calorie": "h,
-    "carbohydrate": "h,
-    "protein": "h,
-    "province": "h,
-    "sugars": "h,
-    "salt": "h,
-    "cholesterol": "h,
-    "saturated_fatty_acids": "h,
-    "trans_fat": "h 
-}</t>
+    <t>[
+    {
+        "id": "3",
+        "food_cd": "D000008",
+        "group_name": "육류구이",
+        "food_name": "닭갈비",
+        "research_year": "2019",
+        "maker_name": "춘천",
+        "ref_name": "외식영양성분자료집 통합본(20122017년)",
+        "serving_size": "300",
+        "calorie": "558.47",
+        "carbohydrate": "23.1",
+        "protein": "45.5",
+        "province": "31.6",
+        "sugars": "8.5",
+        "salt": "1016.94",
+        "cholesterol": "217.67",
+        "saturated_fatty_acids": "11.3",
+        "trans_fat": "0.3"
+    }
+]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조건에 해당하는 음식 정보 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -493,11 +500,12 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
     <col min="7" max="7" width="32.85546875" customWidth="1"/>
@@ -529,21 +537,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="266">
+    <row r="2" spans="1:8" ht="306">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>

</xml_diff>